<commit_message>
Update Database.java / Graduation_Info_List.java / MainActivity.java / LoginActivity.java / design_subject_list.xlsx / required_subject_list.xlsx
removed firebase db dependencies.
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/design_subject_list.xlsx
+++ b/app/src/main/res/raw/design_subject_list.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\knuGra\app\src\main\res\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E201A3-4177-44AF-940F-6A55B906FCF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C1568E-F19D-4073-B41F-72CC881B5E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12181" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="설계과목목록 - 설계과목목록" sheetId="2" r:id="rId1"/>
+    <sheet name="설계과목목록" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -92,19 +92,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
     <font>
       <sz val="8"/>
@@ -113,143 +105,20 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="14"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -258,47 +127,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1460,167 +1290,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:IV10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949093EB-76BD-4020-84DD-520AB99B43A5}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.35546875" defaultRowHeight="19.899999999999999" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="256" width="16.35546875" style="13" customWidth="1"/>
+    <col min="1" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.55" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="25.5">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" ht="25.5">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6">
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:6" ht="25.5">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" ht="25.5">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11">
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:6" ht="25.5">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11">
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:6" ht="25.5">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9" t="s">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:6" ht="25.5">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11">
+      <c r="E7">
         <v>2</v>
       </c>
-      <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:6" ht="38.25">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11">
+      <c r="E8">
         <v>4</v>
       </c>
-      <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:6" ht="38.25">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9" t="s">
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11">
+      <c r="E9">
         <v>4</v>
       </c>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update design_subject_list.xlsx, required_subject_list.xlsx, Graduation_Info_List / subjectname
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/design_subject_list.xlsx
+++ b/app/src/main/res/raw/design_subject_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\knuGra\app\src\main\res\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsungpc\Desktop\SCProject\implementgit\app\src\main\res\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C1568E-F19D-4073-B41F-72CC881B5E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3AE987-F790-4A2A-A53B-CDD98AB3568C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12181" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="936" yWindow="2328" windowWidth="14916" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설계과목목록" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>교과목번호</t>
   </si>
@@ -28,71 +28,85 @@
     <t>개설학과</t>
   </si>
   <si>
+    <t>교과구분</t>
+  </si>
+  <si>
+    <t>학기</t>
+  </si>
+  <si>
+    <t>기초창의공학설계</t>
+  </si>
+  <si>
+    <t>자바프로그래밍</t>
+  </si>
+  <si>
+    <t>시스템프로그래밍</t>
+  </si>
+  <si>
+    <t>소프트웨어설계</t>
+  </si>
+  <si>
+    <t>디지털설계및실험</t>
+  </si>
+  <si>
+    <t>소프트웨어공학</t>
+  </si>
+  <si>
+    <t>종합설계프로젝트1</t>
+  </si>
+  <si>
+    <t>종합설계프로젝트2</t>
+  </si>
+  <si>
+    <t>COMP205</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP217</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ELEC462</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP224</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP225</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP422</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEC401</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEC402</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>교과목명</t>
-  </si>
-  <si>
-    <t>교과구분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>학점</t>
-  </si>
-  <si>
-    <t>학기</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMP205 </t>
-  </si>
-  <si>
-    <t>기초창의공학설계</t>
-  </si>
-  <si>
-    <t>COMP217</t>
-  </si>
-  <si>
-    <t>자바프로그래밍</t>
-  </si>
-  <si>
-    <t>ELEC462</t>
-  </si>
-  <si>
-    <t>시스템프로그래밍</t>
-  </si>
-  <si>
-    <t>COMP224</t>
-  </si>
-  <si>
-    <t>소프트웨어설계</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMP225 </t>
-  </si>
-  <si>
-    <t>디지털설계및실험</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMP422 </t>
-  </si>
-  <si>
-    <t>소프트웨어공학</t>
-  </si>
-  <si>
-    <t>ITEC401</t>
-  </si>
-  <si>
-    <t>종합설계프로젝트1</t>
-  </si>
-  <si>
-    <t>ITEC402</t>
-  </si>
-  <si>
-    <t>종합설계프로젝트2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -101,6 +115,13 @@
     <font>
       <sz val="8"/>
       <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
@@ -127,8 +148,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1294,124 +1318,197 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="6" width="18.140625" customWidth="1"/>
+    <col min="1" max="6" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="25.5">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5">
-      <c r="A3" t="s">
-        <v>8</v>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="25.5">
-      <c r="A4" t="s">
-        <v>10</v>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="25.5">
-      <c r="A5" t="s">
-        <v>12</v>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="25.5">
-      <c r="A6" t="s">
-        <v>14</v>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" ht="25.5">
-      <c r="A7" t="s">
-        <v>16</v>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" ht="38.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" ht="38.25">
-      <c r="A9" t="s">
-        <v>20</v>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E9">
         <v>4</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Graduation_Info_List.java ,xlsx required subject
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/design_subject_list.xlsx
+++ b/app/src/main/res/raw/design_subject_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsungpc\Desktop\SCProject\implementgit\app\src\main\res\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3AE987-F790-4A2A-A53B-CDD98AB3568C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6C9A49-50D3-41D4-B95A-C5419768D542}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="2328" windowWidth="14916" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3948" yWindow="1056" windowWidth="12984" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설계과목목록" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>교과목번호</t>
   </si>
@@ -1318,7 +1318,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1350,15 +1350,11 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2">
         <v>2</v>
       </c>
@@ -1370,9 +1366,7 @@
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -1390,9 +1384,7 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -1410,9 +1402,7 @@
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -1430,9 +1420,7 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -1450,9 +1438,7 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -1470,9 +1456,7 @@
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8" t="s">
         <v>10</v>
       </c>
@@ -1490,9 +1474,7 @@
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Update Database.java fixed null value error
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/design_subject_list.xlsx
+++ b/app/src/main/res/raw/design_subject_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsungpc\Desktop\SCProject\implementgit\app\src\main\res\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6C9A49-50D3-41D4-B95A-C5419768D542}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3AE987-F790-4A2A-A53B-CDD98AB3568C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3948" yWindow="1056" windowWidth="12984" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="936" yWindow="2328" windowWidth="14916" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설계과목목록" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>교과목번호</t>
   </si>
@@ -1318,7 +1318,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1350,11 +1350,15 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E2">
         <v>2</v>
       </c>
@@ -1366,7 +1370,9 @@
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -1384,7 +1390,9 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -1402,7 +1410,9 @@
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -1420,7 +1430,9 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -1438,7 +1450,9 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -1456,7 +1470,9 @@
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
@@ -1474,7 +1490,9 @@
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Update Graduation_Info_List / CareerSuccessFragment / design_subject_list.xlsx / required_subject_list.xlsx
fixed multiple reference
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/design_subject_list.xlsx
+++ b/app/src/main/res/raw/design_subject_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsungpc\Desktop\SCProject\implementgit\app\src\main\res\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\knuGra\app\src\main\res\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3AE987-F790-4A2A-A53B-CDD98AB3568C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD63C53-2F70-4776-AF99-D2E9026DF364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="2328" windowWidth="14916" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12181" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설계과목목록" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>교과목번호</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>학기</t>
-  </si>
-  <si>
-    <t>기초창의공학설계</t>
   </si>
   <si>
     <t>자바프로그래밍</t>
@@ -98,7 +95,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>기초창의공학설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1318,12 +1315,12 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="6" width="18.109375" customWidth="1"/>
+    <col min="1" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1334,13 +1331,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1348,163 +1345,115 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1"/>
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B7" s="1"/>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7">
         <v>2</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8">
         <v>4</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B9" s="1"/>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9">
         <v>4</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>